<commit_message>
Finished adding Test Cases. Also updated some framework pieces to be ready for Chrome support. Finally restructed some folders to module the design.
</commit_message>
<xml_diff>
--- a/XoiSuite/Test Notes.xlsx
+++ b/XoiSuite/Test Notes.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.thomas.ALI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF1BAF1-CC53-4DDC-9CDE-28C31A4BE9F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="48">
   <si>
     <t>Test Scenarios (For Lead Page Form)</t>
   </si>
@@ -162,19 +161,19 @@
     <t>"Please change your e-mail address to continue."</t>
   </si>
   <si>
-    <t>Validate Successful Lead Data (IE)</t>
-  </si>
-  <si>
-    <t>Validate Unsuccessful Lead Data (IE)</t>
-  </si>
-  <si>
-    <t>Validate Lead Page UI Functionality (IE)</t>
+    <t>Notes (Automation)</t>
+  </si>
+  <si>
+    <t>This Test needed to be ordered a littl different for the implementation. Each field requires to have focus taken away to update. So, you instead clear all fields, then validate the errors.</t>
+  </si>
+  <si>
+    <t>Unsuccessful Submit with Wrong Format Required (E-mail)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,7 +216,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -234,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -243,9 +242,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -256,23 +252,29 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -282,41 +284,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,628 +600,643 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="16"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
     </row>
     <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="15"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="14"/>
+      <c r="B10" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>47</v>
+      <c r="A14" s="14" t="s">
+        <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="20"/>
+      <c r="B18" s="17"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="20"/>
+      <c r="B28" s="17"/>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="16"/>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="B37" s="17"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+      <c r="C38" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="C39" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+      <c r="C41" s="14"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="C43" s="14"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="C45" s="14"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+      <c r="C46" s="14"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
+      <c r="C47" s="14"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
       <c r="B48" s="3"/>
     </row>
     <row r="49" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="16"/>
+      <c r="B49" s="17"/>
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+    <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="16"/>
+      <c r="B59" s="17"/>
     </row>
     <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
+    <row r="65" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B69" s="16"/>
+      <c r="B69" s="17"/>
     </row>
     <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B70" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="7"/>
+      <c r="A78" s="6"/>
       <c r="B78" s="1"/>
     </row>
     <row r="79" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B79" s="16"/>
+      <c r="A79" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79" s="17"/>
     </row>
     <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="17"/>
-      <c r="B84" s="1" t="s">
+      <c r="A84" s="12"/>
+      <c r="B84" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="7" t="s">
+      <c r="A85" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="12" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C39:C47"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A83:A84"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A28:B28"/>

</xml_diff>